<commit_message>
Testcase for Profile Info and Tutorial are added now
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Complete Course.xlsx
+++ b/bin/com/NFHS/xls/Complete Course.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17610" windowHeight="5895" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17610" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L11"/>
 </workbook>
 </file>
 
@@ -55,10 +54,10 @@
     <t>Results</t>
   </si>
   <si>
-    <t>testuser1@weboapps.com</t>
-  </si>
-  <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>bhabani.shankar105@weboapps.com</t>
   </si>
   <si>
     <t>pass</t>
@@ -415,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,13 +474,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="43.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="18.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
@@ -507,10 +506,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>

</xml_diff>